<commit_message>
LeetCode p58 p94 p1460
</commit_message>
<xml_diff>
--- a/题目清单.xlsx
+++ b/题目清单.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$9</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="57">
   <si>
     <t>OJ网站</t>
   </si>
@@ -160,6 +160,36 @@
   </si>
   <si>
     <t>找下标规律</t>
+  </si>
+  <si>
+    <t>二叉树的中序遍历</t>
+  </si>
+  <si>
+    <t>dfs,二叉树中序遍历</t>
+  </si>
+  <si>
+    <t>给出二叉树，输出其中序遍历</t>
+  </si>
+  <si>
+    <t>dfs先左子树，再跟节点，后右子树，记录中序遍历最终打印</t>
+  </si>
+  <si>
+    <t>最后一个单词的长度</t>
+  </si>
+  <si>
+    <t>给出只包含单词和空格的字符串，求最后一个单词的长度</t>
+  </si>
+  <si>
+    <t>简单字符串处理</t>
+  </si>
+  <si>
+    <t>通过翻转子数组使两个数组相等</t>
+  </si>
+  <si>
+    <t>给出两个等长数组，判断是否能通过若干次子数组反转使得二者一样</t>
+  </si>
+  <si>
+    <t>冒泡排序就是多次的长度为2的子数组反转，所以只要两个数组内的相应元素个数相等即一定可以达成</t>
   </si>
 </sst>
 </file>
@@ -804,7 +834,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -828,6 +858,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1183,10 +1216,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1453,41 +1486,127 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="4">
         <v>118</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="5">
         <v>44797</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="6" t="s">
         <v>46</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="9"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="7">
+        <v>94</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="9">
+        <v>44797</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="7">
+        <v>58</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="9">
+        <v>44797</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="7"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1460</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="9">
+        <v>44797</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H8">
+  <autoFilter ref="A1:H9">
     <extLst/>
   </autoFilter>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2 E3 E4 E5 E6 E7 E8:E9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2 E3 E4 E5 E6 E7 E8 E9 E10 E11:E12">
       <formula1>"0星,1星,2星,3星,4星,5星"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>